<commit_message>
updated the sheet with some complete status
</commit_message>
<xml_diff>
--- a/FITNESS Testing_Version2.xlsx
+++ b/FITNESS Testing_Version2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\Excel_changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92330B8-73FD-4913-8094-93900B8C5856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Launching" sheetId="5" r:id="rId1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="214">
   <si>
     <t>Scn1</t>
   </si>
@@ -758,11 +759,23 @@
   <si>
     <t>completed</t>
   </si>
+  <si>
+    <t>Need to discuss</t>
+  </si>
+  <si>
+    <t>Developer's Comment</t>
+  </si>
+  <si>
+    <t>Please provide Phone number</t>
+  </si>
+  <si>
+    <t>Please provide Location</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -810,7 +823,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -832,6 +845,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -888,7 +907,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -979,6 +998,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1259,33 +1279,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="23.42578125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="23.44140625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1338,7 +1358,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1354,8 +1374,8 @@
       <c r="E2" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>156</v>
+      <c r="F2" s="19" t="s">
+        <v>157</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -1369,7 +1389,7 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:18" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1386,7 +1406,7 @@
         <v>149</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>156</v>
+        <v>210</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -1400,7 +1420,7 @@
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1416,8 +1436,8 @@
       <c r="E4" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>156</v>
+      <c r="F4" s="19" t="s">
+        <v>157</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1431,7 +1451,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1447,8 +1467,8 @@
       <c r="E5" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>156</v>
+      <c r="F5" s="19" t="s">
+        <v>157</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1462,7 +1482,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1493,7 +1513,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1507,8 +1527,8 @@
         <v>189</v>
       </c>
       <c r="E7" s="7"/>
-      <c r="F7" s="7" t="s">
-        <v>156</v>
+      <c r="F7" s="19" t="s">
+        <v>157</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -1523,7 +1543,7 @@
       <c r="Q7" s="7"/>
       <c r="R7" s="8"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1553,7 +1573,7 @@
       <c r="Q8" s="7"/>
       <c r="R8" s="8"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1578,7 +1598,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1610,36 +1630,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="53.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="15"/>
+    <col min="3" max="3" width="38.88671875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="53.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.44140625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.109375" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
@@ -1653,57 +1674,60 @@
         <v>108</v>
       </c>
       <c r="E1" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="N1" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="O1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="P1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="Q1" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="R1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="S1" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>156</v>
+      <c r="C2" s="18" t="s">
+        <v>157</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>159</v>
@@ -1722,8 +1746,9 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1734,7 +1759,9 @@
         <v>156</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>212</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -1748,21 +1775,22 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>156</v>
+      <c r="C4" s="18" t="s">
+        <v>157</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1776,8 +1804,9 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1788,7 +1817,9 @@
         <v>156</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>213</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -1802,16 +1833,17 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-    </row>
-    <row r="6" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>156</v>
+      <c r="C6" s="18" t="s">
+        <v>157</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>165</v>
@@ -1830,16 +1862,17 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-    </row>
-    <row r="7" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="S6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>156</v>
+      <c r="C7" s="18" t="s">
+        <v>157</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>167</v>
@@ -1858,16 +1891,17 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-    </row>
-    <row r="8" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>156</v>
+      <c r="C8" s="18" t="s">
+        <v>157</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>170</v>
@@ -1886,16 +1920,17 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-    </row>
-    <row r="9" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>156</v>
+      <c r="C9" s="18" t="s">
+        <v>157</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>171</v>
@@ -1914,8 +1949,9 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-    </row>
-    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1942,8 +1978,9 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-    </row>
-    <row r="11" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1968,16 +2005,17 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>156</v>
+      <c r="C12" s="18" t="s">
+        <v>157</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>174</v>
@@ -1996,16 +2034,17 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
-    </row>
-    <row r="13" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>156</v>
+      <c r="C13" s="18" t="s">
+        <v>157</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>178</v>
@@ -2024,16 +2063,17 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
-    </row>
-    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>156</v>
+      <c r="C14" s="18" t="s">
+        <v>157</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>182</v>
@@ -2052,16 +2092,17 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
-    </row>
-    <row r="15" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>156</v>
+      <c r="C15" s="18" t="s">
+        <v>157</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>180</v>
@@ -2080,32 +2121,33 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>3</v>
       </c>
@@ -2161,7 +2203,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="23">
         <v>1</v>
       </c>
@@ -2189,7 +2231,7 @@
       <c r="Q2" s="21"/>
       <c r="R2" s="21"/>
     </row>
-    <row r="3" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A3" s="23">
         <v>2</v>
       </c>
@@ -2217,7 +2259,7 @@
       <c r="Q3" s="21"/>
       <c r="R3" s="21"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2228,11 +2270,11 @@
         <v>67</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E4" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2247,63 +2289,63 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2317,22 +2359,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="76.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>186</v>
       </c>
@@ -2349,7 +2391,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2360,11 +2402,11 @@
       <c r="D2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2375,11 +2417,11 @@
       <c r="D3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2394,63 +2436,63 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2464,33 +2506,33 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="94.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="94.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.42578125" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.44140625" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" customWidth="1"/>
     <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="82.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="82.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>3</v>
       </c>
@@ -2539,7 +2581,7 @@
       </c>
       <c r="Q1" s="27"/>
     </row>
-    <row r="2" spans="1:17" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>9</v>
       </c>
@@ -2568,7 +2610,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>11</v>
       </c>
@@ -2597,7 +2639,7 @@
       <c r="P3" s="28"/>
       <c r="Q3" s="27"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="28" t="s">
         <v>11</v>
       </c>
@@ -2626,7 +2668,7 @@
       <c r="P4" s="28"/>
       <c r="Q4" s="27"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>11</v>
       </c>
@@ -2655,7 +2697,7 @@
       <c r="P5" s="28"/>
       <c r="Q5" s="27"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>11</v>
       </c>
@@ -2684,7 +2726,7 @@
       <c r="P6" s="28"/>
       <c r="Q6" s="27"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="28" t="s">
         <v>11</v>
       </c>
@@ -2711,7 +2753,7 @@
       </c>
       <c r="Q7" s="27"/>
     </row>
-    <row r="8" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28" t="s">
         <v>11</v>
       </c>
@@ -2740,7 +2782,7 @@
       <c r="P8" s="28"/>
       <c r="Q8" s="27"/>
     </row>
-    <row r="9" spans="1:17" ht="48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="48" x14ac:dyDescent="0.3">
       <c r="A9" s="28" t="s">
         <v>11</v>
       </c>
@@ -2767,7 +2809,7 @@
       <c r="P9" s="28"/>
       <c r="Q9" s="27"/>
     </row>
-    <row r="10" spans="1:17" ht="36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="36" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
         <v>11</v>
       </c>
@@ -2794,7 +2836,7 @@
       <c r="P10" s="28"/>
       <c r="Q10" s="27"/>
     </row>
-    <row r="11" spans="1:17" ht="108" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="84" x14ac:dyDescent="0.3">
       <c r="A11" s="28" t="s">
         <v>11</v>
       </c>
@@ -2821,7 +2863,7 @@
       <c r="P11" s="28"/>
       <c r="Q11" s="27"/>
     </row>
-    <row r="12" spans="1:17" ht="48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="48" x14ac:dyDescent="0.3">
       <c r="A12" s="28" t="s">
         <v>11</v>
       </c>
@@ -2858,7 +2900,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="28" t="s">
         <v>11</v>
       </c>
@@ -2897,7 +2939,7 @@
       </c>
       <c r="Q13" s="27"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="28" t="s">
         <v>11</v>
       </c>
@@ -2938,7 +2980,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="36" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
         <v>11</v>
       </c>
@@ -2979,7 +3021,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="A16" s="28" t="s">
         <v>11</v>
       </c>
@@ -3024,7 +3066,7 @@
       </c>
       <c r="Q16" s="27"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
         <v>11</v>
       </c>
@@ -3049,7 +3091,7 @@
       <c r="P17" s="28"/>
       <c r="Q17" s="27"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="28" t="s">
         <v>11</v>
       </c>
@@ -3076,7 +3118,7 @@
       </c>
       <c r="Q18" s="27"/>
     </row>
-    <row r="19" spans="1:17" ht="24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="A19" s="28" t="s">
         <v>11</v>
       </c>
@@ -3103,7 +3145,7 @@
       </c>
       <c r="Q19" s="27"/>
     </row>
-    <row r="20" spans="1:17" ht="48" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="48" x14ac:dyDescent="0.3">
       <c r="A20" s="28" t="s">
         <v>11</v>
       </c>
@@ -3130,7 +3172,7 @@
       </c>
       <c r="Q20" s="27"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="28" t="s">
         <v>11</v>
       </c>
@@ -3155,7 +3197,7 @@
       <c r="P21" s="28"/>
       <c r="Q21" s="27"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="28" t="s">
         <v>11</v>
       </c>
@@ -3182,7 +3224,7 @@
       </c>
       <c r="Q22" s="27"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="28" t="s">
         <v>11</v>
       </c>
@@ -3207,7 +3249,7 @@
       <c r="P23" s="28"/>
       <c r="Q23" s="27"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>11</v>
       </c>
@@ -3234,7 +3276,7 @@
       </c>
       <c r="Q24" s="27"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="s">
         <v>11</v>
       </c>
@@ -3263,15 +3305,15 @@
       </c>
       <c r="Q25" s="27"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="28" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="36" t="s">
-        <v>156</v>
+      <c r="C26" s="29" t="s">
+        <v>157</v>
       </c>
       <c r="D26" s="32"/>
       <c r="E26" s="28"/>
@@ -3290,7 +3332,7 @@
       </c>
       <c r="Q26" s="27"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="27"/>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
@@ -3311,7 +3353,7 @@
       </c>
       <c r="Q27" s="27"/>
     </row>
-    <row r="28" spans="1:17" ht="24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
         <v>37</v>
       </c>
@@ -3334,7 +3376,7 @@
       </c>
       <c r="Q28" s="27"/>
     </row>
-    <row r="29" spans="1:17" ht="24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="27">
         <v>1</v>
       </c>
@@ -3359,7 +3401,7 @@
       </c>
       <c r="Q29" s="27"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="27">
         <v>2</v>
       </c>
@@ -3382,7 +3424,7 @@
       </c>
       <c r="Q30" s="27"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="27">
         <v>3</v>
       </c>
@@ -3407,7 +3449,7 @@
       </c>
       <c r="Q31" s="27"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="27">
         <v>4</v>
       </c>
@@ -3435,27 +3477,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView topLeftCell="C4" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="97.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="97.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -3487,7 +3529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -3515,7 +3557,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -3543,7 +3585,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3571,7 +3613,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -3599,7 +3641,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3618,7 +3660,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3638,7 +3680,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -3653,7 +3695,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -3673,7 +3715,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -3695,7 +3737,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -3715,7 +3757,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="I12" s="4" t="s">
@@ -3725,7 +3767,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I13" s="4" t="s">
         <v>41</v>
       </c>
@@ -3733,7 +3775,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I14" s="4" t="s">
         <v>42</v>
       </c>
@@ -3741,7 +3783,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I15" s="4" t="s">
         <v>43</v>
       </c>
@@ -3749,7 +3791,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I16" s="4" t="s">
         <v>44</v>
       </c>
@@ -3764,28 +3806,28 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="140.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="140.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="47" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="82.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="82.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -3817,7 +3859,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3843,7 +3885,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3866,7 +3908,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3892,7 +3934,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3915,7 +3957,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3938,7 +3980,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -3967,7 +4009,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -3988,28 +4030,28 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="115" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.44140625" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="47" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="82.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="82.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -4041,7 +4083,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4052,7 +4094,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -4081,7 +4123,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -4110,7 +4152,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -4136,14 +4178,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
         <v>116</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="40" t="s">
         <v>156</v>
       </c>
       <c r="D6" t="s">
@@ -4165,7 +4207,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -4194,7 +4236,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -4220,7 +4262,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -4252,7 +4294,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -4284,7 +4326,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -4310,7 +4352,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -4342,7 +4384,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -4371,7 +4413,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>

</xml_diff>